<commit_message>
After a long time
</commit_message>
<xml_diff>
--- a/docs/features.xlsx
+++ b/docs/features.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="25">
   <si>
     <t>Probe SNMP</t>
   </si>
@@ -63,9 +63,6 @@
     <t>Dashboard básico</t>
   </si>
   <si>
-    <t>Probe básica (modelo)</t>
-  </si>
-  <si>
     <t>Interface para administração do banco (campos / triggers)</t>
   </si>
   <si>
@@ -91,6 +88,9 @@
   </si>
   <si>
     <t>-</t>
+  </si>
+  <si>
+    <t>Probe básica (modelo) + Tool Registering</t>
   </si>
 </sst>
 </file>
@@ -470,7 +470,7 @@
   <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -483,7 +483,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>3</v>
@@ -500,7 +500,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -508,7 +508,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -516,7 +516,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -524,7 +524,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -532,7 +532,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -540,7 +540,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -548,7 +548,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -556,7 +556,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -564,7 +564,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -572,7 +572,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -580,87 +580,103 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="4">
-        <v>12</v>
-      </c>
-      <c r="B13" t="s">
-        <v>20</v>
+      <c r="A13" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="4">
-        <v>13</v>
-      </c>
-      <c r="B14" t="s">
+      <c r="A14" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="4">
-        <v>14</v>
-      </c>
-      <c r="B15" t="s">
-        <v>14</v>
+      <c r="A15" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="4">
-        <v>15</v>
-      </c>
-      <c r="B16" t="s">
-        <v>16</v>
+      <c r="A16" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C17" s="3"/>
       <c r="D17" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C18" s="3"/>
       <c r="D18" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C19" s="3"/>
       <c r="D19" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C20" s="3"/>
       <c r="D20" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>